<commit_message>
age and sex correlation
</commit_message>
<xml_diff>
--- a/paper/Tables/Suplemmentary_2.xlsx
+++ b/paper/Tables/Suplemmentary_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hsjdbcn.es\dfsroot\Recursos\metabolismosinaptico\SOFIA\metabolomics_rett_grin\paper\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\killescas\OneDrive - San Juan de Dios\Desktop\GitHub\metabolomics\paper\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,12 +27,6 @@
     <t>Control</t>
   </si>
   <si>
-    <t>RTT</t>
-  </si>
-  <si>
-    <t>p-value RTT</t>
-  </si>
-  <si>
     <t>Hypo-glutamatergic</t>
   </si>
   <si>
@@ -163,6 +157,12 @@
   </si>
   <si>
     <t>Sedoheptulose</t>
+  </si>
+  <si>
+    <t>Hyper-glutamatergic</t>
+  </si>
+  <si>
+    <t>p-value hyper-glutamatergic</t>
   </si>
 </sst>
 </file>
@@ -447,10 +447,16 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75">
       <c r="A1" s="1" t="s">
@@ -460,21 +466,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3">
         <v>1.75981915E-3</v>
@@ -483,18 +489,18 @@
         <v>3.5329597500000001E-3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3">
         <v>3.2469808500000001E-3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3">
         <v>0.17225354500000001</v>
@@ -503,18 +509,18 @@
         <v>3.6895205E-2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3">
         <v>3.6268364999999997E-2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3">
         <v>0.73488085000000003</v>
@@ -523,18 +529,18 @@
         <v>1.3527470500000001</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" s="3">
         <v>1.51469115</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12.75">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>3.4971079999999999</v>
@@ -543,18 +549,18 @@
         <v>2.6713045000000002</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" s="3">
         <v>2.9374579999999999</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.75">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3">
         <v>4.5886055000000014E-3</v>
@@ -563,18 +569,18 @@
         <v>5.8056080000000003E-3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E6" s="3">
         <v>3.6729655E-3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3">
         <v>0.56222972500000001</v>
@@ -583,18 +589,18 @@
         <v>0.215339955</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7" s="3">
         <v>0.18325949499999999</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3">
         <v>5.1882292500000005E-4</v>
@@ -603,18 +609,18 @@
         <v>3.5390502500000002E-4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E8" s="3">
         <v>3.2784742500000002E-4</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="12.75">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3">
         <v>2.0732503499999999E-2</v>
@@ -623,18 +629,18 @@
         <v>4.2056354999999998E-3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E9" s="3">
         <v>2.9805665000000002E-3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3">
         <v>1.2655862500000001E-3</v>
@@ -643,18 +649,18 @@
         <v>3.2432228999999999E-3</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E10" s="3">
         <v>3.66692525E-3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3">
         <v>2.7681127999999999E-2</v>
@@ -663,18 +669,18 @@
         <v>1.2922326E-2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E11" s="3">
         <v>1.1760486000000001E-2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3">
         <v>3.5141129499999999</v>
@@ -683,18 +689,18 @@
         <v>1.41975805</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E12" s="3">
         <v>1.3697580499999999</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3">
         <v>36.837060000000001</v>
@@ -703,18 +709,18 @@
         <v>28.751445</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E13" s="3">
         <v>29.123360000000002</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3">
         <v>38.974597000000003</v>
@@ -723,18 +729,18 @@
         <v>5.7737904999999996</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E14" s="3">
         <v>4.168952</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3">
         <v>18.137313500000001</v>
@@ -743,18 +749,18 @@
         <v>15.293158</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E15" s="3">
         <v>17.507443500000001</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3">
         <v>14.188912999999999</v>
@@ -763,18 +769,18 @@
         <v>10.263913000000001</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E16" s="3">
         <v>11.894041</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="12.75">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="3">
         <v>49.131815000000003</v>
@@ -783,18 +789,18 @@
         <v>41.50909</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E17" s="3">
         <v>48.686365000000002</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="12.75">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="3">
         <v>4.7474657499999999</v>
@@ -803,18 +809,18 @@
         <v>4.3748630500000001</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E18" s="3">
         <v>4.43787675</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="12.75">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3">
         <v>1.4136814</v>
@@ -823,18 +829,18 @@
         <v>0.80986374999999988</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E19" s="3">
         <v>0.6213168</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.75">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20" s="3">
         <v>8.6207925000000003</v>
@@ -843,18 +849,18 @@
         <v>7.6826734999999999</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E20" s="3">
         <v>7.7544555000000006</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="3">
         <v>19.9653995</v>
@@ -863,18 +869,18 @@
         <v>14.945358000000001</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E21" s="3">
         <v>11.4916065</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.75">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="3">
         <v>54.393929999999997</v>
@@ -883,18 +889,18 @@
         <v>40.197544999999998</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E22" s="3">
         <v>41.499869999999987</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12.75">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" s="3">
         <v>30.422889999999999</v>
@@ -903,18 +909,18 @@
         <v>26.722300000000001</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E23" s="3">
         <v>32.197226000000001</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="12.75">
       <c r="A24" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>1.8409091</v>
@@ -923,18 +929,18 @@
         <v>1.0431818500000001</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E24" s="3">
         <v>0.58636359999999998</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="12.75">
       <c r="A25" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3">
         <v>0.89540229999999998</v>
@@ -943,18 +949,18 @@
         <v>0.32049804999999998</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E25" s="3">
         <v>0.38927200000000001</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="12.75">
       <c r="A26" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" s="3">
         <v>3.4815789499999998</v>
@@ -963,18 +969,18 @@
         <v>1.12894735</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E26" s="3">
         <v>0.86578945000000007</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12.75">
       <c r="A27" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B27" s="3">
         <v>0.82790699999999995</v>
@@ -983,18 +989,18 @@
         <v>0.97499999999999998</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E27" s="3">
         <v>0.48255819999999999</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="12.75">
       <c r="A28" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B28" s="3">
         <v>22.590540499999999</v>
@@ -1003,18 +1009,18 @@
         <v>9.0297295000000002</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E28" s="3">
         <v>9.8599104999999998</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="12.75">
       <c r="A29" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B29" s="3">
         <v>0.13255360499999999</v>
@@ -1023,18 +1029,18 @@
         <v>6.8713455000000007E-2</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E29" s="3">
         <v>7.3099415000000001E-2</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="12.75">
       <c r="A30" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" s="3">
         <v>1140.595</v>
@@ -1043,18 +1049,18 @@
         <v>809.02749999999992</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E30" s="3">
         <v>889.55499999999995</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="12.75">
       <c r="A31" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" s="3">
         <v>0.50525905500000001</v>
@@ -1063,18 +1069,18 @@
         <v>0.30950526</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E31" s="3">
         <v>0.20802493499999999</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="12.75">
       <c r="A32" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="3">
         <v>1.871</v>
@@ -1083,18 +1089,18 @@
         <v>1.2955000000000001</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E32" s="3">
         <v>2.1890000000000001</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="12.75">
       <c r="A33" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B33" s="3">
         <v>246.86332999999999</v>
@@ -1103,18 +1109,18 @@
         <v>137.03333000000001</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E33" s="3">
         <v>143.93</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="12.75">
       <c r="A34" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B34" s="3">
         <v>213.577145</v>
@@ -1123,18 +1129,18 @@
         <v>112.652855</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E34" s="3">
         <v>92.848564999999994</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="12.75">
       <c r="A35" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B35" s="3">
         <v>325.62290000000002</v>
@@ -1143,18 +1149,18 @@
         <v>412.53570000000002</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E35" s="3">
         <v>363.27429999999998</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="12.75">
       <c r="A36" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B36" s="3">
         <v>39.338693999999997</v>
@@ -1163,18 +1169,18 @@
         <v>20.774854000000001</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E36" s="3">
         <v>20.041423000000002</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="12.75">
       <c r="A37" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B37" s="3">
         <v>1.06773875</v>
@@ -1183,18 +1189,18 @@
         <v>0.36500975000000002</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E37" s="3">
         <v>0.40789474999999997</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="12.75">
       <c r="A38" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B38" s="3">
         <v>0.58954546000000008</v>
@@ -1203,18 +1209,18 @@
         <v>0.27090909499999999</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E38" s="3">
         <v>0.30863636999999999</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="12.75">
       <c r="A39" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B39" s="3">
         <v>2.6681818499999999</v>
@@ -1223,18 +1229,18 @@
         <v>1.67727275</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E39" s="3">
         <v>2.25909095</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="12.75">
       <c r="A40" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B40" s="3">
         <v>56.501365</v>
@@ -1243,18 +1249,18 @@
         <v>30.495909999999999</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E40" s="3">
         <v>35.835005000000002</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="12.75">
       <c r="A41" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B41" s="3">
         <v>0.80714285000000008</v>
@@ -1263,13 +1269,13 @@
         <v>0.38857140000000001</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E41" s="3">
         <v>0.43571425000000003</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1287,15 +1293,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FACE5D818E5F50479853446EE507747E" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e722f55148bbad8870355d780504b59a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d3de4b96-056f-41d8-923d-53addee4e8b2" xmlns:ns4="4b297ba6-3c75-43f4-b046-b7dedaa9211e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e547858e4e7ab4dfb3f8dcd768a35191" ns3:_="" ns4:_="">
     <xsd:import namespace="d3de4b96-056f-41d8-923d-53addee4e8b2"/>
@@ -1504,32 +1501,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65E25971-D2E8-45B6-B20B-1B98D052EA6F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="4b297ba6-3c75-43f4-b046-b7dedaa9211e"/>
     <ds:schemaRef ds:uri="d3de4b96-056f-41d8-923d-53addee4e8b2"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4b297ba6-3c75-43f4-b046-b7dedaa9211e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20296712-2068-434D-B490-E5808E8E0A0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2077CA72-99BB-4EF1-B505-3B6BD04E93D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1546,4 +1544,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20296712-2068-434D-B490-E5808E8E0A0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>